<commit_message>
fixing consequences of issue #241
Some expressions are considered ambiguous that were previously considered unambiguous.
For this reason, try14.adl moves to shouldfail.
</commit_message>
<xml_diff>
--- a/MirrorMe/Mindmaps.xlsx
+++ b/MirrorMe/Mindmaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" tabRatio="809" activeTab="5"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" tabRatio="809" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Beweringen" sheetId="2" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="onBehalfOf" sheetId="26" r:id="rId10"/>
     <sheet name="pop" sheetId="28" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="157">
   <si>
     <t>7148691</t>
   </si>
@@ -301,9 +301,6 @@
     <t>rechtsfeit</t>
   </si>
   <si>
-    <t>feit </t>
-  </si>
-  <si>
     <t>bloot feit</t>
   </si>
   <si>
@@ -571,6 +568,9 @@
   </si>
   <si>
     <t>Een partij is een natuurlijke persoon of rechtspersoon, die met een of meer andere partijen een overeenkomst heeft.</t>
+  </si>
+  <si>
+    <t>feit</t>
   </si>
 </sst>
 </file>
@@ -1283,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,7 +1295,7 @@
     <col min="3" max="3" width="108" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>25</v>
       </c>
@@ -1311,8 +1311,9 @@
       <c r="E1" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
@@ -1325,9 +1326,12 @@
       <c r="D2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
@@ -1343,8 +1347,12 @@
       <c r="E3" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="6" t="str">
+        <f t="shared" ref="G1:G59" si="0">VLOOKUP(E3,$A$3:$B$61,1,FALSE)</f>
+        <v>Overeenkomst</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>58</v>
       </c>
@@ -1358,8 +1366,12 @@
       <c r="E4" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>partij</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>57</v>
       </c>
@@ -1373,8 +1385,12 @@
       <c r="E5" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>partij</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>42</v>
       </c>
@@ -1382,14 +1398,18 @@
         <v>42</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
@@ -1403,8 +1423,12 @@
         <v>5</v>
       </c>
       <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>66</v>
       </c>
@@ -1414,13 +1438,17 @@
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>77</v>
@@ -1429,8 +1457,12 @@
       <c r="E9" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>rechtsfeit</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>78</v>
       </c>
@@ -1438,769 +1470,981 @@
         <v>78</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D10" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="G10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>feit</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="G11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>feit</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>83</v>
-      </c>
       <c r="D12" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>rechtsfeit</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>89</v>
-      </c>
       <c r="D13" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>rechtsfeit</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="G14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>rechtshandeling </v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="G15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>rechtshandeling </v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="G16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>EenzijdigeRechtshandeling</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="G17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>EenzijdigeRechtshandeling</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="G18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>MeerzijdigeRechtshandeling</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E19" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>MeerzijdigeRechtshandeling</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>98</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="G20" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>feitelijkeHandeling</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="G21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>feitelijkeHandeling</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="G22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>EenzPrivRechtshandling</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="G23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>EenzPrivRechtshandling</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="G24" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>MeerzPrivRechtshandling</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>113</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="G25" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>PrivaatrechtelijkeOvereenkomst</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="G26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>VerbObligOvereenkomst</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="G27" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>VerbObligOvereenkomst</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="G28" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>PrivaatrechtelijkeOvereenkomst</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="G29" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>PrivaatrechtelijkeOvereenkomst</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="G30" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>PrivaatrechtelijkeOvereenkomst</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="G31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>GerEenzPrivRechtshandling</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="G32" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>GerEenzPrivRechtshandling</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="G33" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>GerEenzPrivRechtshandling</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="G34" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>OngEenzPrivRechtshandling</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="G35" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>OngEenzPrivRechtshandling</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="G36" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>EenzPublRechtshandling</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="G37" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>EenzPublRechtshandling</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="G38" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>EenzPublRechtshandling</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="G39" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>WederkerigeOvereenkomst</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="G40" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>WederkerigeOvereenkomst</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="G41" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>EenzijdigeOvereenkomst</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="G42" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>GoederenrechtelijkeOvereenkomst</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="G43" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>GoederenrechtelijkeOvereenkomst</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="G44" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>BevrijdendeLiberatoireOvereenkomst</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="G45" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>BevrijdendeLiberatoireOvereenkomst</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="G46" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>FamilierechtelijkeOvereenkomst</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="G47" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>MeerzPublRechtshandling</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="G48" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>OnrechtmatigeDaad</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="G49" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>OnrechtmatigeDaad</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="G50" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>OnrechtmatigeDaad</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="G51" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>OnrechtmatigeDaad</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="G52" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>OnrechtmatigeDaad</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C53" s="10"/>
       <c r="D53" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="G53" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>OnrechtmatigeDaad</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C54" s="10"/>
       <c r="D54" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="G54" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>RechtmatigeDaad</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="G55" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>RechtmatigeDaad</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="G56" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>RechtmatigeDaad</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="G57" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>blootRechtsfeit</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="G58" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>blootRechtsfeit</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C59" s="10"/>
       <c r="D59" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="G59" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>blootRechtsfeit</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C60" s="10"/>
       <c r="D60" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="G60" t="str">
+        <f>VLOOKUP(E60,$A$3:$B$61,1,FALSE)</f>
+        <v>blootRechtsfeit</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2322,7 +2566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
exposing a mistake for issue #247
</commit_message>
<xml_diff>
--- a/MirrorMe/Mindmaps.xlsx
+++ b/MirrorMe/Mindmaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" tabRatio="809" activeTab="7"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" tabRatio="809"/>
   </bookViews>
   <sheets>
     <sheet name="Beweringen" sheetId="2" r:id="rId1"/>
@@ -801,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2575,11 +2575,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>